<commit_message>
adding crp to script
</commit_message>
<xml_diff>
--- a/Manuscript_items/Table_CVD_predmodels.xlsx
+++ b/Manuscript_items/Table_CVD_predmodels.xlsx
@@ -728,35 +728,35 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1085,7 +1085,7 @@
       <c r="A2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="32">
         <v>2014</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -1111,7 +1111,7 @@
       <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="32">
         <v>2008</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -1137,7 +1137,7 @@
       <c r="A4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="32">
         <v>2007</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -1163,7 +1163,7 @@
       <c r="A5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="32">
         <v>2008</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1189,7 +1189,7 @@
       <c r="A6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="32">
         <v>2003</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1252,16 +1252,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1269,131 +1269,131 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1401,27 +1401,27 @@
       <c r="A20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="11" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
removal of CRP and Reynolds Score
</commit_message>
<xml_diff>
--- a/Manuscript_items/Table_CVD_predmodels.xlsx
+++ b/Manuscript_items/Table_CVD_predmodels.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>USA</t>
   </si>
@@ -367,50 +367,7 @@
 - Smoking status</t>
   </si>
   <si>
-    <t>Reynolds Risk Score for women (Ridker et al.)</t>
-  </si>
-  <si>
-    <t>Reynolds Risk Score for men (Ridker et al.)</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>Appendix C in https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2752381/</t>
-  </si>
-  <si>
-    <t>- Age
-- Sex
-- Systolic blood pressure
-- Total cholesterol
-- HDL-C
-- Smoking status
-- Family history of myocardial infarction
-- hsCRP</t>
-  </si>
-  <si>
     <t>Not stated, but predominantly white</t>
-  </si>
-  <si>
-    <t>95% non-Hispanic White, 2% Black, 1% Hispanic, 1% Asian, 1% Other</t>
-  </si>
-  <si>
-    <t>- Age
-- Sex
-- Systolic blood pressure
-- Total cholesterol
-- HDL-C
-- Smoking status
-- Family history of myocardial infarction
-- hsCRP
-- History of diabetes
-- HbA1c</t>
-  </si>
-  <si>
-    <t>Box, Model B in https://jamanetwork.com/journals/jama/fullarticle/205528</t>
   </si>
   <si>
     <t>SCORE (Conroy et al.)</t>
@@ -1038,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1118,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>69</v>
@@ -1133,82 +1090,30 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="132.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="32">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>43</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="32">
-        <v>2008</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="32">
-        <v>2003</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>